<commit_message>
Update (Working Multiple ASINs)
</commit_message>
<xml_diff>
--- a/consolidated_forecast.xlsx
+++ b/consolidated_forecast.xlsx
@@ -492,7 +492,7 @@
         <v>160.1393199104967</v>
       </c>
       <c r="D2" t="n">
-        <v>221.2861964294511</v>
+        <v>221.0849778471946</v>
       </c>
       <c r="E2" t="n">
         <v>146</v>
@@ -522,13 +522,13 @@
         <v>45634</v>
       </c>
       <c r="B3" t="n">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" t="n">
         <v>140.7101126442642</v>
       </c>
       <c r="D3" t="n">
-        <v>203.9263651953787</v>
+        <v>201.7484654015377</v>
       </c>
       <c r="E3" t="n">
         <v>98</v>
@@ -558,13 +558,13 @@
         <v>45641</v>
       </c>
       <c r="B4" t="n">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" t="n">
         <v>134.305057165544</v>
       </c>
       <c r="D4" t="n">
-        <v>198.9184621413842</v>
+        <v>195.5400274973452</v>
       </c>
       <c r="E4" t="n">
         <v>90</v>
@@ -594,13 +594,13 @@
         <v>45648</v>
       </c>
       <c r="B5" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C5" t="n">
         <v>137.1143504031909</v>
       </c>
       <c r="D5" t="n">
-        <v>196.0693780496692</v>
+        <v>199.8839534004867</v>
       </c>
       <c r="E5" t="n">
         <v>107</v>
@@ -630,13 +630,13 @@
         <v>45655</v>
       </c>
       <c r="B6" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C6" t="n">
         <v>136.0710800611095</v>
       </c>
       <c r="D6" t="n">
-        <v>195.6479329656704</v>
+        <v>201.3808662571929</v>
       </c>
       <c r="E6" t="n">
         <v>87</v>
@@ -666,13 +666,13 @@
         <v>45662</v>
       </c>
       <c r="B7" t="n">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" t="n">
         <v>127.2728176039879</v>
       </c>
       <c r="D7" t="n">
-        <v>191.8930890981957</v>
+        <v>185.1395569624067</v>
       </c>
       <c r="E7" t="n">
         <v>81</v>
@@ -708,7 +708,7 @@
         <v>118.8715555085086</v>
       </c>
       <c r="D8" t="n">
-        <v>182.5715966257648</v>
+        <v>181.6949562513354</v>
       </c>
       <c r="E8" t="n">
         <v>82</v>
@@ -744,7 +744,7 @@
         <v>117.09426260854</v>
       </c>
       <c r="D9" t="n">
-        <v>179.7323953914248</v>
+        <v>179.616336125509</v>
       </c>
       <c r="E9" t="n">
         <v>80</v>
@@ -774,13 +774,13 @@
         <v>45683</v>
       </c>
       <c r="B10" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" t="n">
         <v>116.1682451285496</v>
       </c>
       <c r="D10" t="n">
-        <v>177.783185057803</v>
+        <v>175.7337833657078</v>
       </c>
       <c r="E10" t="n">
         <v>79</v>
@@ -816,7 +816,7 @@
         <v>106.8112368444398</v>
       </c>
       <c r="D11" t="n">
-        <v>168.0504804117747</v>
+        <v>167.4459777250811</v>
       </c>
       <c r="E11" t="n">
         <v>82</v>
@@ -846,13 +846,13 @@
         <v>45697</v>
       </c>
       <c r="B12" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" t="n">
         <v>92.0746914114978</v>
       </c>
       <c r="D12" t="n">
-        <v>155.5529428207891</v>
+        <v>152.3396702761764</v>
       </c>
       <c r="E12" t="n">
         <v>89</v>
@@ -882,13 +882,13 @@
         <v>45704</v>
       </c>
       <c r="B13" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C13" t="n">
         <v>87.8319741674655</v>
       </c>
       <c r="D13" t="n">
-        <v>150.9217107908434</v>
+        <v>153.6437735335704</v>
       </c>
       <c r="E13" t="n">
         <v>88</v>
@@ -918,13 +918,13 @@
         <v>45711</v>
       </c>
       <c r="B14" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C14" t="n">
         <v>104.0665901788299</v>
       </c>
       <c r="D14" t="n">
-        <v>164.3183949962696</v>
+        <v>165.7719481597741</v>
       </c>
       <c r="E14" t="n">
         <v>83</v>
@@ -954,13 +954,13 @@
         <v>45718</v>
       </c>
       <c r="B15" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C15" t="n">
         <v>129.0963392672726</v>
       </c>
       <c r="D15" t="n">
-        <v>190.2767027514267</v>
+        <v>190.8652103296676</v>
       </c>
       <c r="E15" t="n">
         <v>80</v>
@@ -990,13 +990,13 @@
         <v>45725</v>
       </c>
       <c r="B16" t="n">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" t="n">
         <v>138.2451720905276</v>
       </c>
       <c r="D16" t="n">
-        <v>202.8766063644528</v>
+        <v>200.4464218693634</v>
       </c>
       <c r="E16" t="n">
         <v>82</v>
@@ -1026,13 +1026,13 @@
         <v>45732</v>
       </c>
       <c r="B17" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C17" t="n">
         <v>119.9330063967863</v>
       </c>
       <c r="D17" t="n">
-        <v>182.110049628758</v>
+        <v>185.9286942386037</v>
       </c>
       <c r="E17" t="n">
         <v>81</v>
@@ -1068,7 +1068,7 @@
         <v>89.81249305448448</v>
       </c>
       <c r="D18" t="n">
-        <v>153.9503301893685</v>
+        <v>155.2100107058579</v>
       </c>
       <c r="E18" t="n">
         <v>76</v>
@@ -1098,13 +1098,13 @@
         <v>45746</v>
       </c>
       <c r="B19" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" t="n">
         <v>75.53401683205507</v>
       </c>
       <c r="D19" t="n">
-        <v>135.4445690493043</v>
+        <v>133.6299565829612</v>
       </c>
       <c r="E19" t="n">
         <v>73</v>
@@ -1134,13 +1134,13 @@
         <v>45753</v>
       </c>
       <c r="B20" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C20" t="n">
         <v>88.04697620922246</v>
       </c>
       <c r="D20" t="n">
-        <v>149.4079188499079</v>
+        <v>154.4480246787629</v>
       </c>
       <c r="E20" t="n">
         <v>81</v>
@@ -1176,7 +1176,7 @@
         <v>110.9702056577835</v>
       </c>
       <c r="D21" t="n">
-        <v>177.036367668138</v>
+        <v>176.4309099129671</v>
       </c>
       <c r="E21" t="n">
         <v>72</v>
@@ -1283,7 +1283,7 @@
         <v>166.4751861498553</v>
       </c>
       <c r="D2" t="n">
-        <v>234.3468343449142</v>
+        <v>234.0890616412142</v>
       </c>
       <c r="E2" t="n">
         <v>174</v>
@@ -1313,13 +1313,13 @@
         <v>45634</v>
       </c>
       <c r="B3" t="n">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C3" t="n">
         <v>180.8397447646376</v>
       </c>
       <c r="D3" t="n">
-        <v>249.5076491481891</v>
+        <v>255.5624876177054</v>
       </c>
       <c r="E3" t="n">
         <v>105</v>
@@ -1355,7 +1355,7 @@
         <v>154.0090714360897</v>
       </c>
       <c r="D4" t="n">
-        <v>226.6255649450782</v>
+        <v>228.1469955562823</v>
       </c>
       <c r="E4" t="n">
         <v>86</v>
@@ -1385,13 +1385,13 @@
         <v>45648</v>
       </c>
       <c r="B5" t="n">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C5" t="n">
         <v>105.3601955580259</v>
       </c>
       <c r="D5" t="n">
-        <v>180.7028828754909</v>
+        <v>171.0383102333376</v>
       </c>
       <c r="E5" t="n">
         <v>105</v>
@@ -1421,13 +1421,13 @@
         <v>45655</v>
       </c>
       <c r="B6" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" t="n">
         <v>64.84919566925181</v>
       </c>
       <c r="D6" t="n">
-        <v>137.2923843478614</v>
+        <v>129.1274725553662</v>
       </c>
       <c r="E6" t="n">
         <v>83</v>
@@ -1457,13 +1457,13 @@
         <v>45662</v>
       </c>
       <c r="B7" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="n">
         <v>48.89471581103997</v>
       </c>
       <c r="D7" t="n">
-        <v>118.8660328383326</v>
+        <v>121.9366143077742</v>
       </c>
       <c r="E7" t="n">
         <v>67</v>
@@ -1499,7 +1499,7 @@
         <v>53.08408112802231</v>
       </c>
       <c r="D8" t="n">
-        <v>123.7919232877161</v>
+        <v>122.4787996547277</v>
       </c>
       <c r="E8" t="n">
         <v>71</v>
@@ -1529,13 +1529,13 @@
         <v>45676</v>
       </c>
       <c r="B9" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C9" t="n">
         <v>63.19006356021882</v>
       </c>
       <c r="D9" t="n">
-        <v>133.2448155376883</v>
+        <v>138.1457550133834</v>
       </c>
       <c r="E9" t="n">
         <v>66</v>
@@ -1565,13 +1565,13 @@
         <v>45683</v>
       </c>
       <c r="B10" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C10" t="n">
         <v>68.60224395789895</v>
       </c>
       <c r="D10" t="n">
-        <v>141.3399672337405</v>
+        <v>142.975817229278</v>
       </c>
       <c r="E10" t="n">
         <v>65</v>
@@ -1601,13 +1601,13 @@
         <v>45690</v>
       </c>
       <c r="B11" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C11" t="n">
         <v>65.9676905849193</v>
       </c>
       <c r="D11" t="n">
-        <v>141.5139094011011</v>
+        <v>130.5190494994928</v>
       </c>
       <c r="E11" t="n">
         <v>62</v>
@@ -1637,13 +1637,13 @@
         <v>45697</v>
       </c>
       <c r="B12" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C12" t="n">
         <v>55.90581604176235</v>
       </c>
       <c r="D12" t="n">
-        <v>123.1563236719524</v>
+        <v>129.8849263716982</v>
       </c>
       <c r="E12" t="n">
         <v>68</v>
@@ -1673,13 +1673,13 @@
         <v>45704</v>
       </c>
       <c r="B13" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" t="n">
         <v>41.45379216004909</v>
       </c>
       <c r="D13" t="n">
-        <v>111.8809033529902</v>
+        <v>116.591158556338</v>
       </c>
       <c r="E13" t="n">
         <v>69</v>
@@ -1715,7 +1715,7 @@
         <v>29.02486284422996</v>
       </c>
       <c r="D14" t="n">
-        <v>103.0672500213886</v>
+        <v>100.7306759217145</v>
       </c>
       <c r="E14" t="n">
         <v>66</v>
@@ -1745,13 +1745,13 @@
         <v>45718</v>
       </c>
       <c r="B15" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" t="n">
         <v>25.79464953480029</v>
       </c>
       <c r="D15" t="n">
-        <v>93.30304830104535</v>
+        <v>98.98452153795701</v>
       </c>
       <c r="E15" t="n">
         <v>62</v>
@@ -1781,13 +1781,13 @@
         <v>45725</v>
       </c>
       <c r="B16" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="n">
         <v>32.72261470460429</v>
       </c>
       <c r="D16" t="n">
-        <v>105.0662604173101</v>
+        <v>101.3594400008375</v>
       </c>
       <c r="E16" t="n">
         <v>63</v>
@@ -1823,7 +1823,7 @@
         <v>41.68677369843287</v>
       </c>
       <c r="D17" t="n">
-        <v>109.8690980712604</v>
+        <v>110.3852022442807</v>
       </c>
       <c r="E17" t="n">
         <v>62</v>
@@ -1853,13 +1853,13 @@
         <v>45739</v>
       </c>
       <c r="B18" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" t="n">
         <v>43.1172197491487</v>
       </c>
       <c r="D18" t="n">
-        <v>115.4354479669998</v>
+        <v>114.247613863925</v>
       </c>
       <c r="E18" t="n">
         <v>59</v>
@@ -1889,13 +1889,13 @@
         <v>45746</v>
       </c>
       <c r="B19" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" t="n">
         <v>37.28832950554266</v>
       </c>
       <c r="D19" t="n">
-        <v>103.3528651153817</v>
+        <v>107.9919638190198</v>
       </c>
       <c r="E19" t="n">
         <v>56</v>
@@ -1931,7 +1931,7 @@
         <v>35.35349654581896</v>
       </c>
       <c r="D20" t="n">
-        <v>103.9339010223012</v>
+        <v>104.796324783441</v>
       </c>
       <c r="E20" t="n">
         <v>65</v>
@@ -1961,13 +1961,13 @@
         <v>45760</v>
       </c>
       <c r="B21" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C21" t="n">
         <v>46.74881781857644</v>
       </c>
       <c r="D21" t="n">
-        <v>113.7417464556093</v>
+        <v>119.8240781494048</v>
       </c>
       <c r="E21" t="n">
         <v>57</v>
@@ -2074,7 +2074,7 @@
         <v>-1.514556315933952</v>
       </c>
       <c r="D2" t="n">
-        <v>18.5068253544142</v>
+        <v>17.64042441662114</v>
       </c>
       <c r="E2" t="n">
         <v>5</v>
@@ -2104,13 +2104,13 @@
         <v>45634</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>-2.617230251045018</v>
       </c>
       <c r="D3" t="n">
-        <v>18.28912198569227</v>
+        <v>16.6201965439883</v>
       </c>
       <c r="E3" t="n">
         <v>6</v>
@@ -2146,7 +2146,7 @@
         <v>-2.91510982750959</v>
       </c>
       <c r="D4" t="n">
-        <v>15.71118446627673</v>
+        <v>16.6548992654382</v>
       </c>
       <c r="E4" t="n">
         <v>7</v>
@@ -2182,7 +2182,7 @@
         <v>-2.47419129882358</v>
       </c>
       <c r="D5" t="n">
-        <v>17.34332442219636</v>
+        <v>16.75117441384114</v>
       </c>
       <c r="E5" t="n">
         <v>8</v>
@@ -2212,13 +2212,13 @@
         <v>45655</v>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>-2.293697859405471</v>
       </c>
       <c r="D6" t="n">
-        <v>16.32923647152826</v>
+        <v>18.22392699872321</v>
       </c>
       <c r="E6" t="n">
         <v>6</v>
@@ -2254,7 +2254,7 @@
         <v>-3.409903982860305</v>
       </c>
       <c r="D7" t="n">
-        <v>15.46173247856318</v>
+        <v>15.89800956019089</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
@@ -2290,7 +2290,7 @@
         <v>-5.426062413872022</v>
       </c>
       <c r="D8" t="n">
-        <v>13.47369897396437</v>
+        <v>12.93572156289842</v>
       </c>
       <c r="E8" t="n">
         <v>6</v>
@@ -2326,7 +2326,7 @@
         <v>-6.514999184766452</v>
       </c>
       <c r="D9" t="n">
-        <v>12.44978366091885</v>
+        <v>11.85865455729252</v>
       </c>
       <c r="E9" t="n">
         <v>6</v>
@@ -2356,13 +2356,13 @@
         <v>45683</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
         <v>-5.356960383649724</v>
       </c>
       <c r="D10" t="n">
-        <v>12.61968107785234</v>
+        <v>14.31037386445029</v>
       </c>
       <c r="E10" t="n">
         <v>5</v>
@@ -2392,13 +2392,13 @@
         <v>45690</v>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="n">
         <v>-2.805807977619671</v>
       </c>
       <c r="D11" t="n">
-        <v>16.4813544672036</v>
+        <v>18.24644518752616</v>
       </c>
       <c r="E11" t="n">
         <v>6</v>
@@ -2434,7 +2434,7 @@
         <v>-1.084684004065017</v>
       </c>
       <c r="D12" t="n">
-        <v>17.96331634289257</v>
+        <v>18.08077902055489</v>
       </c>
       <c r="E12" t="n">
         <v>5</v>
@@ -2464,13 +2464,13 @@
         <v>45704</v>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
         <v>-1.392526154904137</v>
       </c>
       <c r="D13" t="n">
-        <v>17.95385736010364</v>
+        <v>18.7823393435219</v>
       </c>
       <c r="E13" t="n">
         <v>5</v>
@@ -2506,7 +2506,7 @@
         <v>-2.950978700796204</v>
       </c>
       <c r="D14" t="n">
-        <v>18.09728059204943</v>
+        <v>15.78982458671447</v>
       </c>
       <c r="E14" t="n">
         <v>5</v>
@@ -2542,7 +2542,7 @@
         <v>-4.631948961416269</v>
       </c>
       <c r="D15" t="n">
-        <v>15.09143938835147</v>
+        <v>13.93146918752713</v>
       </c>
       <c r="E15" t="n">
         <v>5</v>
@@ -2578,7 +2578,7 @@
         <v>-6.742286704585696</v>
       </c>
       <c r="D16" t="n">
-        <v>13.55344231345545</v>
+        <v>11.23525802650791</v>
       </c>
       <c r="E16" t="n">
         <v>6</v>
@@ -2614,7 +2614,7 @@
         <v>-10.26842404528771</v>
       </c>
       <c r="D17" t="n">
-        <v>10.7013329536713</v>
+        <v>8.771486893698055</v>
       </c>
       <c r="E17" t="n">
         <v>6</v>
@@ -2650,7 +2650,7 @@
         <v>-14.56307683371668</v>
       </c>
       <c r="D18" t="n">
-        <v>2.510289731372714</v>
+        <v>5.785366465743787</v>
       </c>
       <c r="E18" t="n">
         <v>5</v>
@@ -2686,7 +2686,7 @@
         <v>-17.06484829811482</v>
       </c>
       <c r="D19" t="n">
-        <v>2.947625900475655</v>
+        <v>3.351765655209337</v>
       </c>
       <c r="E19" t="n">
         <v>4</v>
@@ -2722,7 +2722,7 @@
         <v>-16.15716449908831</v>
       </c>
       <c r="D20" t="n">
-        <v>3.828621137750378</v>
+        <v>3.492528385869525</v>
       </c>
       <c r="E20" t="n">
         <v>5</v>
@@ -2758,7 +2758,7 @@
         <v>-13.64580245057114</v>
       </c>
       <c r="D21" t="n">
-        <v>5.662621612379652</v>
+        <v>5.506021936574759</v>
       </c>
       <c r="E21" t="n">
         <v>4</v>
@@ -2865,7 +2865,7 @@
         <v>152.4554252729202</v>
       </c>
       <c r="D2" t="n">
-        <v>191.4144174618348</v>
+        <v>190.0910339471775</v>
       </c>
       <c r="E2" t="n">
         <v>104</v>
@@ -2895,13 +2895,13 @@
         <v>45634</v>
       </c>
       <c r="B3" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C3" t="n">
         <v>195.1748744888661</v>
       </c>
       <c r="D3" t="n">
-        <v>230.638589256635</v>
+        <v>233.3275293256467</v>
       </c>
       <c r="E3" t="n">
         <v>67</v>
@@ -2931,13 +2931,13 @@
         <v>45641</v>
       </c>
       <c r="B4" t="n">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C4" t="n">
         <v>200.216905685073</v>
       </c>
       <c r="D4" t="n">
-        <v>234.2046755780689</v>
+        <v>240.8982021110415</v>
       </c>
       <c r="E4" t="n">
         <v>60</v>
@@ -2967,13 +2967,13 @@
         <v>45648</v>
       </c>
       <c r="B5" t="n">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" t="n">
         <v>165.6138375330004</v>
       </c>
       <c r="D5" t="n">
-        <v>206.2250480492322</v>
+        <v>203.2885980182523</v>
       </c>
       <c r="E5" t="n">
         <v>68</v>
@@ -3003,13 +3003,13 @@
         <v>45655</v>
       </c>
       <c r="B6" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C6" t="n">
         <v>125.2903206893107</v>
       </c>
       <c r="D6" t="n">
-        <v>162.4066031865327</v>
+        <v>162.8886632926573</v>
       </c>
       <c r="E6" t="n">
         <v>55</v>
@@ -3045,7 +3045,7 @@
         <v>108.2391577836601</v>
       </c>
       <c r="D7" t="n">
-        <v>145.778868942673</v>
+        <v>146.8522370952435</v>
       </c>
       <c r="E7" t="n">
         <v>53</v>
@@ -3081,7 +3081,7 @@
         <v>108.9587251086184</v>
       </c>
       <c r="D8" t="n">
-        <v>147.4189044716754</v>
+        <v>146.537376583008</v>
       </c>
       <c r="E8" t="n">
         <v>54</v>
@@ -3111,13 +3111,13 @@
         <v>45676</v>
       </c>
       <c r="B9" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="n">
         <v>105.9050127804263</v>
       </c>
       <c r="D9" t="n">
-        <v>141.9529185457743</v>
+        <v>141.0210774705989</v>
       </c>
       <c r="E9" t="n">
         <v>52</v>
@@ -3153,7 +3153,7 @@
         <v>98.43921378240555</v>
       </c>
       <c r="D10" t="n">
-        <v>136.2936685104605</v>
+        <v>136.1640153028027</v>
       </c>
       <c r="E10" t="n">
         <v>51</v>
@@ -3183,13 +3183,13 @@
         <v>45690</v>
       </c>
       <c r="B11" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" t="n">
         <v>107.9051862151046</v>
       </c>
       <c r="D11" t="n">
-        <v>148.5052123286437</v>
+        <v>146.252532241961</v>
       </c>
       <c r="E11" t="n">
         <v>54</v>
@@ -3225,7 +3225,7 @@
         <v>139.7750056808643</v>
       </c>
       <c r="D12" t="n">
-        <v>178.6808169980723</v>
+        <v>175.5692787002968</v>
       </c>
       <c r="E12" t="n">
         <v>63</v>
@@ -3261,7 +3261,7 @@
         <v>161.925826857676</v>
       </c>
       <c r="D13" t="n">
-        <v>199.525825663797</v>
+        <v>200.029598337419</v>
       </c>
       <c r="E13" t="n">
         <v>62</v>
@@ -3291,13 +3291,13 @@
         <v>45711</v>
       </c>
       <c r="B14" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C14" t="n">
         <v>137.2814296358182</v>
       </c>
       <c r="D14" t="n">
-        <v>174.1076501092204</v>
+        <v>176.6062986051131</v>
       </c>
       <c r="E14" t="n">
         <v>61</v>
@@ -3327,13 +3327,13 @@
         <v>45718</v>
       </c>
       <c r="B15" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C15" t="n">
         <v>74.91938631222418</v>
       </c>
       <c r="D15" t="n">
-        <v>111.1136996715692</v>
+        <v>116.1634683976632</v>
       </c>
       <c r="E15" t="n">
         <v>59</v>
@@ -3369,7 +3369,7 @@
         <v>30.88385624800652</v>
       </c>
       <c r="D16" t="n">
-        <v>67.09970927942314</v>
+        <v>68.45867424498672</v>
       </c>
       <c r="E16" t="n">
         <v>59</v>
@@ -3405,7 +3405,7 @@
         <v>48.26294095546403</v>
       </c>
       <c r="D17" t="n">
-        <v>83.4090116316423</v>
+        <v>83.86851019117597</v>
       </c>
       <c r="E17" t="n">
         <v>59</v>
@@ -3441,7 +3441,7 @@
         <v>105.5419904717432</v>
       </c>
       <c r="D18" t="n">
-        <v>145.187794561479</v>
+        <v>144.5568439352778</v>
       </c>
       <c r="E18" t="n">
         <v>56</v>
@@ -3477,7 +3477,7 @@
         <v>138.6671491667557</v>
       </c>
       <c r="D19" t="n">
-        <v>176.3171266723292</v>
+        <v>176.2469300397337</v>
       </c>
       <c r="E19" t="n">
         <v>55</v>
@@ -3513,7 +3513,7 @@
         <v>113.8976213917097</v>
       </c>
       <c r="D20" t="n">
-        <v>153.6132183226802</v>
+        <v>152.7115243547536</v>
       </c>
       <c r="E20" t="n">
         <v>61</v>
@@ -3549,7 +3549,7 @@
         <v>64.46966010339058</v>
       </c>
       <c r="D21" t="n">
-        <v>101.9866369065423</v>
+        <v>103.5775184397716</v>
       </c>
       <c r="E21" t="n">
         <v>54</v>
@@ -3656,7 +3656,7 @@
         <v>-22.12577319336522</v>
       </c>
       <c r="D2" t="n">
-        <v>-11.75703877713515</v>
+        <v>-12.0649011511458</v>
       </c>
       <c r="E2" t="n">
         <v>28</v>
@@ -3692,7 +3692,7 @@
         <v>-70.61697148788227</v>
       </c>
       <c r="D3" t="n">
-        <v>-60.89847029904524</v>
+        <v>-58.60255706277554</v>
       </c>
       <c r="E3" t="n">
         <v>27</v>
@@ -3728,7 +3728,7 @@
         <v>-92.87850469802409</v>
       </c>
       <c r="D4" t="n">
-        <v>-82.5657156685884</v>
+        <v>-82.17838698355609</v>
       </c>
       <c r="E4" t="n">
         <v>17</v>
@@ -3764,7 +3764,7 @@
         <v>-41.59667064398767</v>
       </c>
       <c r="D5" t="n">
-        <v>-31.20877989308915</v>
+        <v>-30.02321168508124</v>
       </c>
       <c r="E5" t="n">
         <v>20</v>
@@ -3800,7 +3800,7 @@
         <v>75.22508882576415</v>
       </c>
       <c r="D6" t="n">
-        <v>85.74472895046475</v>
+        <v>85.62308419655966</v>
       </c>
       <c r="E6" t="n">
         <v>15</v>
@@ -3836,7 +3836,7 @@
         <v>175.3478135360106</v>
       </c>
       <c r="D7" t="n">
-        <v>186.1953639870356</v>
+        <v>186.0589138553771</v>
       </c>
       <c r="E7" t="n">
         <v>16</v>
@@ -3872,7 +3872,7 @@
         <v>169.295295131984</v>
       </c>
       <c r="D8" t="n">
-        <v>179.1192745216059</v>
+        <v>179.9279473612815</v>
       </c>
       <c r="E8" t="n">
         <v>16</v>
@@ -3908,7 +3908,7 @@
         <v>58.78632180888359</v>
       </c>
       <c r="D9" t="n">
-        <v>70.1320687267006</v>
+        <v>69.74082401413624</v>
       </c>
       <c r="E9" t="n">
         <v>16</v>
@@ -3944,7 +3944,7 @@
         <v>-46.278773008698</v>
       </c>
       <c r="D10" t="n">
-        <v>-35.53221435455279</v>
+        <v>-35.82501465321602</v>
       </c>
       <c r="E10" t="n">
         <v>16</v>
@@ -3980,7 +3980,7 @@
         <v>-32.35409084554779</v>
       </c>
       <c r="D11" t="n">
-        <v>-21.84880343133083</v>
+        <v>-21.41693286155797</v>
       </c>
       <c r="E11" t="n">
         <v>17</v>
@@ -4010,13 +4010,13 @@
         <v>45697</v>
       </c>
       <c r="B12" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C12" t="n">
         <v>92.53522946072407</v>
       </c>
       <c r="D12" t="n">
-        <v>102.3673684508703</v>
+        <v>103.1766388522287</v>
       </c>
       <c r="E12" t="n">
         <v>16</v>
@@ -4052,7 +4052,7 @@
         <v>196.8682518270654</v>
       </c>
       <c r="D13" t="n">
-        <v>207.0726140987557</v>
+        <v>207.2844332072682</v>
       </c>
       <c r="E13" t="n">
         <v>16</v>
@@ -4088,7 +4088,7 @@
         <v>164.7025628841462</v>
       </c>
       <c r="D14" t="n">
-        <v>175.1525590425176</v>
+        <v>175.877213565638</v>
       </c>
       <c r="E14" t="n">
         <v>15</v>
@@ -4118,13 +4118,13 @@
         <v>45718</v>
       </c>
       <c r="B15" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" t="n">
         <v>28.3267233726577</v>
       </c>
       <c r="D15" t="n">
-        <v>38.4256380656872</v>
+        <v>39.32749247658997</v>
       </c>
       <c r="E15" t="n">
         <v>16</v>
@@ -4160,7 +4160,7 @@
         <v>-60.04122128416662</v>
       </c>
       <c r="D16" t="n">
-        <v>-49.68505910582507</v>
+        <v>-50.14715971954683</v>
       </c>
       <c r="E16" t="n">
         <v>17</v>
@@ -4190,13 +4190,13 @@
         <v>45732</v>
       </c>
       <c r="B17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="n">
         <v>4.261183091194372</v>
       </c>
       <c r="D17" t="n">
-        <v>15.38804637448898</v>
+        <v>14.84852449256483</v>
       </c>
       <c r="E17" t="n">
         <v>16</v>
@@ -4226,13 +4226,13 @@
         <v>45739</v>
       </c>
       <c r="B18" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C18" t="n">
         <v>157.4304685519537</v>
       </c>
       <c r="D18" t="n">
-        <v>168.1601295481196</v>
+        <v>167.6023283419961</v>
       </c>
       <c r="E18" t="n">
         <v>16</v>
@@ -4268,7 +4268,7 @@
         <v>233.7692723560557</v>
       </c>
       <c r="D19" t="n">
-        <v>244.3164679000932</v>
+        <v>244.121833014396</v>
       </c>
       <c r="E19" t="n">
         <v>15</v>
@@ -4304,7 +4304,7 @@
         <v>148.752406610352</v>
       </c>
       <c r="D20" t="n">
-        <v>159.2673809210679</v>
+        <v>160.1105965927824</v>
       </c>
       <c r="E20" t="n">
         <v>18</v>
@@ -4340,7 +4340,7 @@
         <v>-7.948342930574016</v>
       </c>
       <c r="D21" t="n">
-        <v>3.046537611419986</v>
+        <v>2.525499866017072</v>
       </c>
       <c r="E21" t="n">
         <v>16</v>
@@ -4387,17 +4387,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Product Title</t>
+          <t>product title</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Week</t>
+          <t>week</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>year</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">

</xml_diff>